<commit_message>
Fix " comptabilite avance " in " fichier taxe " rappel issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_6_2023.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_6_2023.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,13 +415,13 @@
         <v>Taxe/avance</v>
       </c>
       <c r="L1" t="str">
+        <v>MT brut (Rappel)</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Taxe (Rappel)</v>
+      </c>
+      <c r="N1" t="str">
         <v>Caution</v>
-      </c>
-      <c r="M1" t="str">
-        <v>MT brut (Rappel)</v>
-      </c>
-      <c r="N1" t="str">
-        <v>Taxe (Rappel)</v>
       </c>
       <c r="O1" t="str">
         <v>MT net</v>
@@ -429,54 +429,336 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>988/DIRECTION CAPITAL SOFT</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C2" t="str">
+        <v>B12346</v>
+      </c>
+      <c r="D2" t="str">
+        <v>BAKKALI MOHAMED</v>
+      </c>
+      <c r="E2" t="str">
+        <v>non</v>
+      </c>
+      <c r="F2" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="str">
+        <v>--</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="str">
+        <v>--</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>10000</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="str">
+        <v>--</v>
+      </c>
+      <c r="O2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>988/DIRECTION CAPITAL SOFT</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C3" t="str">
+        <v>A123456</v>
+      </c>
+      <c r="D3" t="str">
+        <v>YOUSSEF</v>
+      </c>
+      <c r="E3" t="str">
+        <v>non</v>
+      </c>
+      <c r="F3" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3" t="str">
+        <v>--</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="str">
+        <v>--</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>20000</v>
+      </c>
+      <c r="M3">
+        <v>2000</v>
+      </c>
+      <c r="N3" t="str">
+        <v>--</v>
+      </c>
+      <c r="O3">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>988/DIRECTION CAPITAL SOFT</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C4" t="str">
+        <v>J207703</v>
+      </c>
+      <c r="D4" t="str">
+        <v>ACHENGLI LAILA</v>
+      </c>
+      <c r="E4" t="str">
+        <v>non</v>
+      </c>
+      <c r="F4" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
+        <v>--</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <v>--</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>10000</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="str">
+        <v>--</v>
+      </c>
+      <c r="O4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>988/DIRECTION CAPITAL SOFT</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C5" t="str">
+        <v>B12346</v>
+      </c>
+      <c r="D5" t="str">
+        <v>BAKKALI MOHAMED</v>
+      </c>
+      <c r="E5" t="str">
+        <v>non</v>
+      </c>
+      <c r="F5" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>2000</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>20000</v>
+      </c>
+      <c r="O5">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>988/DIRECTION CAPITAL SOFT</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C6" t="str">
+        <v>A123456</v>
+      </c>
+      <c r="D6" t="str">
+        <v>YOUSSEF</v>
+      </c>
+      <c r="E6" t="str">
+        <v>non</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>4000</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>400</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>40000</v>
+      </c>
+      <c r="O6">
+        <v>43600</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>988/DIRECTION CAPITAL SOFT</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C7" t="str">
+        <v>J207703</v>
+      </c>
+      <c r="D7" t="str">
+        <v>ACHENGLI LAILA</v>
+      </c>
+      <c r="E7" t="str">
+        <v>non</v>
+      </c>
+      <c r="F7" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>2000</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>20000</v>
+      </c>
+      <c r="O7">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B2" t="str">
+      <c r="B8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C2" t="str">
+      <c r="C8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D2" t="str">
+      <c r="D8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E2" t="str">
+      <c r="E8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F2" t="str">
+      <c r="F8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G2" t="str">
+      <c r="G8" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
+      <c r="H8">
+        <v>8000</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>400</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>40000</v>
+      </c>
+      <c r="M8">
+        <v>2000</v>
+      </c>
+      <c r="N8">
+        <v>80000</v>
+      </c>
+      <c r="O8">
+        <v>125600</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>